<commit_message>
Ruoli e Regole - Menu
</commit_message>
<xml_diff>
--- a/ClickTab.Web/Resources/Menu.xlsx
+++ b/ClickTab.Web/Resources/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\ClickTab.Workspace\ClickTab.Web\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851F2068-561A-4A28-A4FA-8661283530FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1002E11E-2B8F-4448-AA7B-2E14F4043326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>registry</t>
+  </si>
+  <si>
+    <t>Utenti</t>
+  </si>
+  <si>
+    <t>Ruoli</t>
+  </si>
+  <si>
+    <t>/registry/list-roles</t>
+  </si>
+  <si>
+    <t>/registry/list-users</t>
   </si>
 </sst>
 </file>
@@ -442,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,32 +565,80 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F5" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
-    </row>
-    <row r="21" spans="3:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C21"/>
-      <c r="H21"/>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E31" s="3"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="A5">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="22" spans="3:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C22"/>
+      <c r="H22"/>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E32" s="3"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -588,6 +648,7 @@
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -603,13 +664,22 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Menu e Regole Sotto gruppi
</commit_message>
<xml_diff>
--- a/ClickTab.Web/Resources/Menu.xlsx
+++ b/ClickTab.Web/Resources/Menu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\ClickTab.Workspace\ClickTab.Web\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5A9A7A-E48F-4941-8BDA-E49ED428E319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6490189A-8205-4DCA-BCCB-0BC6F691845E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="1590" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>fa fa-table</t>
+  </si>
+  <si>
+    <t>Sotto Gruppi</t>
+  </si>
+  <si>
+    <t>/tables/list-subcategories</t>
   </si>
 </sst>
 </file>
@@ -453,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,6 +686,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Menu totlte url dal Parent
</commit_message>
<xml_diff>
--- a/ClickTab.Web/Resources/Menu.xlsx
+++ b/ClickTab.Web/Resources/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\ClickTab.Workspace\ClickTab.Web\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA40F41-F7D3-48CE-BD5E-7C227CBBBB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30819808-074B-4354-8F6C-BAE93AEA053E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Deleted</t>
   </si>
   <si>
-    <t>registry</t>
-  </si>
-  <si>
     <t>Utenti</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
   </si>
   <si>
     <t>Gruppi</t>
-  </si>
-  <si>
-    <t>tables</t>
   </si>
   <si>
     <t>fa fa-table</t>
@@ -468,7 +462,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,9 +557,6 @@
       <c r="F3">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
       <c r="I3">
         <v>0</v>
       </c>
@@ -581,10 +572,10 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -593,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -610,10 +601,10 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>20</v>
@@ -622,7 +613,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -639,19 +630,16 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1">
         <v>30</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -668,10 +656,10 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7">
         <v>30</v>
@@ -680,7 +668,7 @@
         <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -697,10 +685,10 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>30</v>
@@ -709,7 +697,7 @@
         <v>32</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -726,10 +714,10 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9">
         <v>30</v>
@@ -738,7 +726,7 @@
         <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>